<commit_message>
Update BOM and PCB with new package sizes
</commit_message>
<xml_diff>
--- a/Altium/BOM.xlsx
+++ b/Altium/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeinzBoehmer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeinzBoehmer/Documents/2018-2019/Second Semester/ECEN 4620/PoC/Altium/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -173,27 +173,6 @@
     <t>https://www.digikey.com/product-detail/en/kemet/C1206C105K3RACTU/399-1255-1-ND/411530</t>
   </si>
   <si>
-    <t>0201</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/LQP03TN2N4B02D/490-6724-1-ND/5802372</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/LQP03TG1N5B02D/490-14701-1-ND/6606307</t>
-  </si>
-  <si>
-    <t>0402</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/LQG15HS27NJ02D/490-2628-1-ND/662908</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/L-07C7N5JV6T/712-1463-1-ND/1915242</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/L-07C6N8JV6T/712-1419-1-ND/1840097</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/bourns-inc/SRR1208-682KL/SRR1208-682KLCT-ND/3974112</t>
   </si>
   <si>
@@ -203,18 +182,6 @@
     <t>https://www.digikey.com/product-detail/en/bourns-inc/CRT1206-BY-1003ELF/CRT1206-BY-1003ELFCT-ND/1775052</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GJM1555C1H1R1BB01D/490-8084-1-ND/4380370</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/500R07S3R6BV4T/712-1164-1-ND/1786626</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GJM1555C1H6R2CB01D/490-3105-1-ND/702371</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/500R07S3R0BV4T/712-1282-1-ND/1786744</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL31A226KQHNNNE/1276-1308-1-ND/3889394</t>
   </si>
   <si>
@@ -227,16 +194,54 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/LQP03TN2N0C02D/490-5553-1-ND/2357652</t>
+    <t>https://www.digikey.com/products/en?keywords=490-1166-1-nd</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/abracon-llc/AIMC-0805-27NJ-T/535-11561-1-ND/2782804</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/american-technical-ceramics/600F6R2BT250XT/1284-1072-1-ND/3905441</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/abracon-llc/AIMC-0805-6N8J-T/535-11573-1-ND/2782797</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL31C030CBCNNNC/1276-2798-1-ND/3890884</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/american-technical-ceramics/600F1R1BT250XT/1284-1028-1-ND/3905408</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en/inductors-coils-chokes/fixed-inductors/71?k=14721-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/abracon-llc/AIMC-0805-1N5S-T/535-11558-1-ND/2782789</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/L-14W2N0CV4E/712-1618-1-ND/6612954</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/american-technical-ceramics/600F3R6BT250XT/1284-1057-1-ND/3905430</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -260,13 +265,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +623,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="102" zoomScalePageLayoutView="102" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -631,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -647,7 +655,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -664,7 +672,7 @@
       <c r="B3" s="3">
         <v>1206</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>7</v>
       </c>
       <c r="D3" t="s">
@@ -676,23 +684,23 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4">
+        <v>52</v>
+      </c>
+      <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>58</v>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" s="3">
         <v>1206</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -706,7 +714,7 @@
       <c r="B6" s="3">
         <v>1206</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
@@ -718,23 +726,23 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7">
+        <v>52</v>
+      </c>
+      <c r="C7" s="6">
         <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>59</v>
+      <c r="E7" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B8" s="3">
         <v>1206</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" t="s">
@@ -746,37 +754,37 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9">
+        <v>52</v>
+      </c>
+      <c r="C9" s="6">
         <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>60</v>
+      <c r="E9" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6">
         <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>61</v>
+      <c r="E10" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" s="3">
         <v>1206</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>6</v>
       </c>
       <c r="D11" t="s">
@@ -790,7 +798,7 @@
       <c r="B12" s="3">
         <v>1206</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" t="s">
@@ -804,28 +812,28 @@
       <c r="B13" s="3">
         <v>1206</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6">
         <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -833,100 +841,100 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
+      <c r="E15" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16">
+        <v>52</v>
+      </c>
+      <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
+      <c r="E16" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17">
+        <v>56</v>
+      </c>
+      <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>66</v>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>52</v>
+      <c r="E18" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19">
+        <v>56</v>
+      </c>
+      <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>53</v>
+      <c r="E19" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20">
+        <v>52</v>
+      </c>
+      <c r="C20" s="6">
         <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
+      <c r="E20" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6">
         <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -936,21 +944,21 @@
       <c r="B22" s="3">
         <v>1206</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -961,7 +969,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>1</v>
       </c>
       <c r="D24" t="s">
@@ -975,7 +983,7 @@
       <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" t="s">
@@ -989,7 +997,7 @@
       <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" t="s">
@@ -1003,7 +1011,7 @@
       <c r="A27" t="s">
         <v>11</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>1</v>
       </c>
       <c r="D27" t="s">
@@ -1017,8 +1025,8 @@
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="C28">
-        <v>1</v>
+      <c r="C28" s="6">
+        <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>38</v>
@@ -1026,5 +1034,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update BOM with in-stock parts
</commit_message>
<xml_diff>
--- a/Altium/BOM.xlsx
+++ b/Altium/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeinzBoehmer/Documents/2018-2019/Second Semester/ECEN 4620/PoC/Altium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HeinzBoehmer/Documents/2018-2019/Second Semester/ECEN 4620/CDR/Altium/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -134,9 +134,6 @@
     <t>48MHz Oscillator</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/abracon-llc/ASV-48.000MHZ-E-T/535-10086-2-ND/2060854</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/abracon-llc/AB38T-32.768KHZ/535-9034-ND/675229</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>https://www.digikey.com/product-detail/en/avx-corporation/12065A2R7CAT2A/478-1461-1-ND/564493</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/kemet/C1206C104K5RAC7867/399-1249-1-ND/411524</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/kemet/C1206C105K3RACTU/399-1255-1-ND/411530</t>
   </si>
   <si>
@@ -228,6 +222,12 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/american-technical-ceramics/600F3R6BT250XT/1284-1057-1-ND/3905430</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ASV-48.000MHZ-E-T/535-10086-1-ND/2060881</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/C1206F104K1RAC7800/399-5113-1-ND/1465638</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="102" zoomScalePageLayoutView="102" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -662,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -679,12 +679,12 @@
         <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
@@ -693,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -707,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -721,12 +721,12 @@
         <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6">
         <v>2</v>
@@ -735,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -749,12 +749,12 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -763,12 +763,12 @@
         <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -777,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -791,7 +791,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -805,7 +805,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -819,12 +819,12 @@
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
@@ -833,7 +833,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -841,7 +841,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6">
         <v>3</v>
@@ -850,12 +850,12 @@
         <v>7</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -864,12 +864,12 @@
         <v>24</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -878,12 +878,12 @@
         <v>25</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -892,12 +892,12 @@
         <v>26</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
@@ -906,12 +906,12 @@
         <v>27</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
@@ -920,12 +920,12 @@
         <v>28</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -934,7 +934,7 @@
         <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -951,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -976,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -990,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1004,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make PCB a much cooler shape and do some other actually important stuff (temperature removal and LED addition)
</commit_message>
<xml_diff>
--- a/Altium/BOM.xlsx
+++ b/Altium/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Comment</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/C1206F104K1RAC7800/399-5113-1-ND/1465638</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCP1206FTD180R/RNCP1206FTD180RCT-ND/2240658</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC1206FR-07220RL/311-220FRCT-ND/731640</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stanley-electric-co/PG1101W-TR/404-1046-1-ND/428848</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stanley-electric-co/BR1101W-TR/404-1042-1-ND/428853</t>
   </si>
 </sst>
 </file>
@@ -265,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -275,6 +293,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="102" zoomScalePageLayoutView="102" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -955,80 +979,136 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>9</v>
+      <c r="B23" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
       </c>
+      <c r="D23" s="7">
+        <v>180</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>33</v>
+      <c r="B24" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
-        <v>4</v>
+      <c r="D24" s="7">
+        <v>220</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
+        <v>69</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C32" s="6">
         <v>2</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>